<commit_message>
Fixed finding a specific month when multiple months are in the db. Added docs and tests.
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="193">
   <si>
     <t xml:space="preserve">Date of shift</t>
   </si>
@@ -31,21 +31,297 @@
     <t xml:space="preserve">Shift end</t>
   </si>
   <si>
+    <t xml:space="preserve">01/03/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06:06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/03/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/03/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06:37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/03/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/03/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/03/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15/03/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16/03/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17/03/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19/03/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06:24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21/03/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09:17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22/03/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23/03/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24/03/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06:31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26/03/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28/03/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09:57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29/03/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20:52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31/03/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/04/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04/04/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/04/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/04/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/04/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/04/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/04/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13/04/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14/04/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16/04/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06:32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18/04/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19/04/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21/04/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22/04/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24/04/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06:28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25/04/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28/04/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29/04/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:26</t>
+  </si>
+  <si>
     <t xml:space="preserve">01/05/19</t>
   </si>
   <si>
-    <t xml:space="preserve">06:10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14:57</t>
-  </si>
-  <si>
     <t xml:space="preserve">02/05/19</t>
   </si>
   <si>
-    <t xml:space="preserve">21:52</t>
-  </si>
-  <si>
     <t xml:space="preserve">06:22</t>
   </si>
   <si>
@@ -61,30 +337,18 @@
     <t xml:space="preserve">05/05/19</t>
   </si>
   <si>
-    <t xml:space="preserve">21:51</t>
-  </si>
-  <si>
     <t xml:space="preserve">06:27</t>
   </si>
   <si>
     <t xml:space="preserve">06/05/19</t>
   </si>
   <si>
-    <t xml:space="preserve">21:50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06:31</t>
-  </si>
-  <si>
     <t xml:space="preserve">08/05/19</t>
   </si>
   <si>
     <t xml:space="preserve">13:00</t>
   </si>
   <si>
-    <t xml:space="preserve">22:03</t>
-  </si>
-  <si>
     <t xml:space="preserve">09/05/19</t>
   </si>
   <si>
@@ -97,18 +361,12 @@
     <t xml:space="preserve">11/05/19</t>
   </si>
   <si>
-    <t xml:space="preserve">06:06</t>
-  </si>
-  <si>
     <t xml:space="preserve">13:43</t>
   </si>
   <si>
     <t xml:space="preserve">12/05/19</t>
   </si>
   <si>
-    <t xml:space="preserve">06:28</t>
-  </si>
-  <si>
     <t xml:space="preserve">14/05/19</t>
   </si>
   <si>
@@ -139,9 +397,6 @@
     <t xml:space="preserve">18/05/19</t>
   </si>
   <si>
-    <t xml:space="preserve">21:48</t>
-  </si>
-  <si>
     <t xml:space="preserve">06:16</t>
   </si>
   <si>
@@ -151,9 +406,6 @@
     <t xml:space="preserve">21:54</t>
   </si>
   <si>
-    <t xml:space="preserve">06:30</t>
-  </si>
-  <si>
     <t xml:space="preserve">21/05/19</t>
   </si>
   <si>
@@ -208,9 +460,6 @@
     <t xml:space="preserve">28/05/19</t>
   </si>
   <si>
-    <t xml:space="preserve">14:36</t>
-  </si>
-  <si>
     <t xml:space="preserve">30/05/19</t>
   </si>
   <si>
@@ -218,6 +467,138 @@
   </si>
   <si>
     <t xml:space="preserve">10:07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06:29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19:52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28/06/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30/06/19</t>
   </si>
 </sst>
 </file>
@@ -297,7 +678,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -318,18 +699,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E66" activeCellId="0" sqref="E66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -411,62 +789,62 @@
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>36</v>
@@ -477,73 +855,73 @@
         <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>53</v>
@@ -565,52 +943,690 @@
         <v>57</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>